<commit_message>
feat: implement grid search, rate limiting, and dynamic file sorting
</commit_message>
<xml_diff>
--- a/datascrapper/united_states/new_york/new_york/gyms.xlsx
+++ b/datascrapper/united_states/new_york/new_york/gyms.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -407,50 +407,68 @@
         <v>Name</v>
       </c>
       <c r="B1" t="str">
-        <v>Google Maps URL</v>
+        <v>Website</v>
       </c>
       <c r="C1" t="str">
+        <v>Contact Number</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Email Address</v>
+      </c>
+      <c r="E1" t="str">
         <v>Rating</v>
       </c>
-      <c r="D1" t="str">
-        <v>Website</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Phone</v>
+      <c r="F1" t="str">
+        <v>LatLong</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Address</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>GÜDSPORT at ARENA ONE</v>
+        <v>Powerhouse Gym 158 W. 27th Street Manhattan</v>
       </c>
       <c r="B2" t="str">
-        <v>https://www.google.com/maps/place/G%C3%9CDSPORT+at+ARENA+ONE/@40.7330929,-74.0345539,13z/data=!3m1!5s0x89c25a19f1335beb:0xad0170a731cdc4b0!4m9!1m2!2m1!1sGyms+in+New+York,+New+York,+United+States!3m5!1s0x89c259d1a4d187a3:0x6c1bfe49ff32a1d0!8m2!3d40.7110759!4d-74.0120239!16s%2Fg%2F11sv00nvhc?entry=ttu&amp;g_ep=EgoyMDI2MDExMy4wIKXMDSoKLDEwMDc5MjA2OUgBUAM%3D</v>
+        <v>https://www.powerhousegymnyc.com/</v>
       </c>
       <c r="C2" t="str">
-        <v/>
+        <v>(646) 429-9278</v>
       </c>
       <c r="D2" t="str">
-        <v>https://www.gudsport.net/</v>
-      </c>
-      <c r="E2" t="str">
-        <v>+1 917-554-4490</v>
+        <v/>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="str">
+        <v>40.746199999999995, -73.9934323</v>
+      </c>
+      <c r="G2" t="str">
+        <v>158 W 27th St, New York, NY 10001, USA</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>MCC Fitness</v>
+        <v>GYM NYC</v>
       </c>
       <c r="B3" t="str">
-        <v>https://www.google.com/maps/place/MCC+Fitness/@40.7330929,-74.0345539,13z/data=!4m9!1m2!2m1!1sGyms+in+New+York,+New+York,+United+States!3m5!1s0x89c25bba56b05583:0x5eada7efd798679b!8m2!3d40.7139708!4d-73.9883747!16s%2Fg%2F11sj5lprt7?entry=ttu&amp;g_ep=EgoyMDI2MDExMy4wIKXMDSoKLDEwMDc5MjA2OUgBUAM%3D</v>
+        <v>http://thegym.nyc/</v>
       </c>
       <c r="C3" t="str">
-        <v/>
+        <v>(646) 678-4723</v>
       </c>
       <c r="D3" t="str">
-        <v>https://mannycantor.org/fitness</v>
-      </c>
-      <c r="E3" t="str">
-        <v>+1 646-395-4285</v>
+        <v/>
+      </c>
+      <c r="E3">
+        <v>4.6</v>
+      </c>
+      <c r="F3" t="str">
+        <v>40.7226743, -73.99611329999999</v>
+      </c>
+      <c r="G3" t="str">
+        <v>227 Mulberry St, New York, NY 10012, USA</v>
       </c>
     </row>
     <row r="4">
@@ -458,55 +476,1338 @@
         <v>GYM NYC East 3rd St.</v>
       </c>
       <c r="B4" t="str">
-        <v>https://www.google.com/maps/place/GYM+NYC+East+3rd+St./@40.7330929,-74.0345539,13z/data=!4m10!1m2!2m1!1sGyms+in+New+York,+New+York,+United+States!3m6!1s0x89c2597f7c3f75e1:0xbb8ce550f8c66e48!8m2!3d40.7235652!4d-73.98483!15sCilHeW1zIGluIE5ldyBZb3JrLCBOZXcgWW9yaywgVW5pdGVkIFN0YXRlc1opIidneW1zIGluIG5ldyB5b3JrIG5ldyB5b3JrIHVuaXRlZCBzdGF0ZXOSAQNneW2aASNDaFpEU1VoTk1HOW5TMFZKUTBGblNVTXhjMlJVU1VkM0VBReABAPoBBAgAEEg!16s%2Fg%2F11sz8c2kgl?entry=ttu&amp;g_ep=EgoyMDI2MDExMy4wIKXMDSoKLDEwMDc5MjA2OUgBUAM%3D</v>
+        <v>http://e3gym.nyc/</v>
       </c>
       <c r="C4" t="str">
-        <v/>
+        <v>(646) 678-5005</v>
       </c>
       <c r="D4" t="str">
-        <v>http://e3gym.nyc/</v>
-      </c>
-      <c r="E4" t="str">
-        <v>+1 646-678-5005</v>
+        <v/>
+      </c>
+      <c r="E4">
+        <v>4.8</v>
+      </c>
+      <c r="F4" t="str">
+        <v>40.723565199999996, -73.98483</v>
+      </c>
+      <c r="G4" t="str">
+        <v>155 E 3rd St, New York, NY 10009, USA</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>GYM NYC</v>
+        <v>Planet Fitness</v>
       </c>
       <c r="B5" t="str">
-        <v>https://www.google.com/maps/place/GYM+NYC/@40.7330929,-74.0345539,13z/data=!4m10!1m2!2m1!1sGyms+in+New+York,+New+York,+United+States!3m6!1s0x89c2598f3597444d:0x235a85560800e250!8m2!3d40.7226743!4d-73.9961133!15sCilHeW1zIGluIE5ldyBZb3JrLCBOZXcgWW9yaywgVW5pdGVkIFN0YXRlc1opIidneW1zIGluIG5ldyB5b3JrIG5ldyB5b3JrIHVuaXRlZCBzdGF0ZXOSAQNneW3gAQA!16s%2Fg%2F11c0w84q0s?entry=ttu&amp;g_ep=EgoyMDI2MDExMy4wIKXMDSoKLDEwMDc5MjA2OUgBUAM%3D</v>
+        <v>https://www.planetfitness.com/gyms/manhattan-herald-square-ny?utm_medium=organic&amp;utm_source=extnet</v>
       </c>
       <c r="C5" t="str">
-        <v/>
+        <v>(646) 518-0330</v>
       </c>
       <c r="D5" t="str">
-        <v>http://thegym.nyc/</v>
-      </c>
-      <c r="E5" t="str">
-        <v>+1 646-678-4723</v>
+        <v/>
+      </c>
+      <c r="E5">
+        <v>3.7</v>
+      </c>
+      <c r="F5" t="str">
+        <v>40.7518576, -73.99105639999999</v>
+      </c>
+      <c r="G5" t="str">
+        <v>215 W 35th St, New York, NY 10001, USA</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
+        <v>GYM NYC Lexington</v>
+      </c>
+      <c r="B6" t="str">
+        <v>https://gym-nyc.com/</v>
+      </c>
+      <c r="C6" t="str">
+        <v>(646) 308-0192</v>
+      </c>
+      <c r="D6" t="str">
+        <v/>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="str">
+        <v>40.7447337, -73.98133829999999</v>
+      </c>
+      <c r="G6" t="str">
+        <v>131 E 31st St, New York, NY 10016, USA</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
         <v>Solace New York</v>
       </c>
-      <c r="B6" t="str">
-        <v>https://www.google.com/maps/place/GYM+NYC/@40.7330929,-74.0345539,13z/data=!4m10!1m2!2m1!1sGyms+in+New+York,+New+York,+United+States!3m6!1s0x89c2598f3597444d:0x235a85560800e250!8m2!3d40.7226743!4d-73.9961133!15sCilHeW1zIGluIE5ldyBZb3JrLCBOZXcgWW9yaywgVW5pdGVkIFN0YXRlc1opIidneW1zIGluIG5ldyB5b3JrIG5ldyB5b3JrIHVuaXRlZCBzdGF0ZXOSAQNneW3gAQA!16s%2Fg%2F11c0w84q0s?entry=ttu&amp;g_ep=EgoyMDI2MDExMy4wIKXMDSoKLDEwMDc5MjA2OUgBUAM%3D</v>
-      </c>
-      <c r="C6" t="str">
-        <v/>
-      </c>
-      <c r="D6" t="str">
-        <v>http://thegym.nyc/</v>
-      </c>
-      <c r="E6" t="str">
-        <v>+1 646-678-4723</v>
+      <c r="B7" t="str">
+        <v>http://www.solacenewyork.com/</v>
+      </c>
+      <c r="C7" t="str">
+        <v>(212) 301-2766</v>
+      </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
+      <c r="E7">
+        <v>4.8</v>
+      </c>
+      <c r="F7" t="str">
+        <v>40.7459869, -73.9831542</v>
+      </c>
+      <c r="G7" t="str">
+        <v>38 E 32nd St, New York, NY 10016, USA</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Chelsea Piers Fitness</v>
+      </c>
+      <c r="B8" t="str">
+        <v>https://fitness.chelseapiers.com/locations/chelsea-ny?utm_source=Google&amp;utm_medium=Listing&amp;utm_campaign=chelseafitness</v>
+      </c>
+      <c r="C8" t="str">
+        <v>(212) 336-6000</v>
+      </c>
+      <c r="D8" t="str">
+        <v/>
+      </c>
+      <c r="E8">
+        <v>4.4</v>
+      </c>
+      <c r="F8" t="str">
+        <v>40.746645, -74.01005700000002</v>
+      </c>
+      <c r="G8" t="str">
+        <v>60 Chelsea Piers, New York, NY 10011, USA</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>GYM NYC BK</v>
+      </c>
+      <c r="B9" t="str">
+        <v>https://gym-nyc.com/</v>
+      </c>
+      <c r="C9" t="str">
+        <v>(646) 688-0366</v>
+      </c>
+      <c r="D9" t="str">
+        <v/>
+      </c>
+      <c r="E9">
+        <v>4.7</v>
+      </c>
+      <c r="F9" t="str">
+        <v>40.6915696, -73.9905785</v>
+      </c>
+      <c r="G9" t="str">
+        <v>85 Livingston St, Brooklyn, NY 11201, USA</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>TMPL Fitness</v>
+      </c>
+      <c r="B10" t="str">
+        <v>https://www.tmplclubs.com/locations/tmpl-avenue-a?utm_source=google&amp;utm_medium=organic&amp;utm_campaign=google_my_business&amp;utm_id=ave_a</v>
+      </c>
+      <c r="C10" t="str">
+        <v>(917) 720-4869</v>
+      </c>
+      <c r="D10" t="str">
+        <v/>
+      </c>
+      <c r="E10">
+        <v>4.9</v>
+      </c>
+      <c r="F10" t="str">
+        <v>40.7232469, -73.9853726</v>
+      </c>
+      <c r="G10" t="str">
+        <v>28-30 Avenue A, New York, NY 10009, USA</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Planet Fitness</v>
+      </c>
+      <c r="B11" t="str">
+        <v>https://www.planetfitness.com/gyms/manhattan-midtown-west-ny?utm_medium=organic&amp;utm_source=extnet</v>
+      </c>
+      <c r="C11" t="str">
+        <v>(212) 336-0750</v>
+      </c>
+      <c r="D11" t="str">
+        <v/>
+      </c>
+      <c r="E11">
+        <v>3.9</v>
+      </c>
+      <c r="F11" t="str">
+        <v>40.76735, -73.98776</v>
+      </c>
+      <c r="G11" t="str">
+        <v>423 W 55th St, New York, NY 10019, USA</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Life Time One Wall Street</v>
+      </c>
+      <c r="B12" t="str">
+        <v>https://www.lifetime.life/locations/ny/one-wall-street.html?utm_source=google&amp;utm_medium=local&amp;utm_campaign=google-local-club</v>
+      </c>
+      <c r="C12" t="str">
+        <v>(212) 671-7100</v>
+      </c>
+      <c r="D12" t="str">
+        <v/>
+      </c>
+      <c r="E12">
+        <v>4.3</v>
+      </c>
+      <c r="F12" t="str">
+        <v>40.7067803, -74.0120018</v>
+      </c>
+      <c r="G12" t="str">
+        <v>29 New St, New York, NY 10005, USA</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>The Strength Club NYC</v>
+      </c>
+      <c r="B13" t="str">
+        <v>https://www.thestrengthclub.com/</v>
+      </c>
+      <c r="C13" t="str">
+        <v/>
+      </c>
+      <c r="D13" t="str">
+        <v/>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13" t="str">
+        <v>40.7446197, -73.9868379</v>
+      </c>
+      <c r="G13" t="str">
+        <v>1 E 28th St # 5b, New York, NY 10016, USA</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Iron Oasis</v>
+      </c>
+      <c r="B14" t="str">
+        <v>https://www.ironoasisnyc.com/</v>
+      </c>
+      <c r="C14" t="str">
+        <v>(845) 595-8411</v>
+      </c>
+      <c r="D14" t="str">
+        <v/>
+      </c>
+      <c r="E14">
+        <v>4.9</v>
+      </c>
+      <c r="F14" t="str">
+        <v>40.752836900000005, -73.9923274</v>
+      </c>
+      <c r="G14" t="str">
+        <v>261 W 35th St, New York, NY 10001, USA</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Crunch Fitness - 54th Street</v>
+      </c>
+      <c r="B15" t="str">
+        <v>https://www.crunch.com/locations/w-54th-st</v>
+      </c>
+      <c r="C15" t="str">
+        <v>(212) 307-7760</v>
+      </c>
+      <c r="D15" t="str">
+        <v/>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" t="str">
+        <v>40.7643104, -73.9835317</v>
+      </c>
+      <c r="G15" t="str">
+        <v>250 W 54th St, New York, NY 10019, USA</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Powerhouse Gym Long Island City</v>
+      </c>
+      <c r="B16" t="str">
+        <v>https://www.powerhousegymlic.net/</v>
+      </c>
+      <c r="C16" t="str">
+        <v>(347) 937-3030</v>
+      </c>
+      <c r="D16" t="str">
+        <v/>
+      </c>
+      <c r="E16">
+        <v>4.7</v>
+      </c>
+      <c r="F16" t="str">
+        <v>40.7511444, -73.9335708</v>
+      </c>
+      <c r="G16" t="str">
+        <v>30-30 Northern Blvd, Long Island City, NY 11101, USA</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>24 Hour Fitness</v>
+      </c>
+      <c r="B17" t="str">
+        <v>https://www.24hourfitness.com/gyms/pelham-manor-ny/pelham-manor-super-sport?Adb_id=GGL_LOC_ACQ_CDP</v>
+      </c>
+      <c r="C17" t="str">
+        <v>(914) 229-3042</v>
+      </c>
+      <c r="D17" t="str">
+        <v/>
+      </c>
+      <c r="E17">
+        <v>3.9</v>
+      </c>
+      <c r="F17" t="str">
+        <v>40.8923959, -73.821018</v>
+      </c>
+      <c r="G17" t="str">
+        <v>887 Pelham Pkwy, Pelham, NY 10803, USA</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Mid City Gym &amp; Tanning</v>
+      </c>
+      <c r="B18" t="str">
+        <v>https://midcitygym.com/</v>
+      </c>
+      <c r="C18" t="str">
+        <v>(212) 757-0850</v>
+      </c>
+      <c r="D18" t="str">
+        <v/>
+      </c>
+      <c r="E18">
+        <v>4.2</v>
+      </c>
+      <c r="F18" t="str">
+        <v>40.758403699999995, -73.9915542</v>
+      </c>
+      <c r="G18" t="str">
+        <v>345 W 42nd St, New York, NY 10036, USA</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Gym U NYC</v>
+      </c>
+      <c r="B19" t="str">
+        <v>http://gymunyc.com/</v>
+      </c>
+      <c r="C19" t="str">
+        <v>(646) 410-2858</v>
+      </c>
+      <c r="D19" t="str">
+        <v/>
+      </c>
+      <c r="E19">
+        <v>4.1</v>
+      </c>
+      <c r="F19" t="str">
+        <v>40.7445928, -73.9961144</v>
+      </c>
+      <c r="G19" t="str">
+        <v>215 W 23rd St, New York, NY 10011, USA</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Life Time</v>
+      </c>
+      <c r="B20" t="str">
+        <v>https://www.lifetime.life/locations/ny/noho.html?utm_source=google&amp;utm_medium=local&amp;utm_campaign=google-local-club</v>
+      </c>
+      <c r="C20" t="str">
+        <v>(917) 438-0300</v>
+      </c>
+      <c r="D20" t="str">
+        <v/>
+      </c>
+      <c r="E20">
+        <v>3.7</v>
+      </c>
+      <c r="F20" t="str">
+        <v>40.7290474, -73.9911669</v>
+      </c>
+      <c r="G20" t="str">
+        <v>62 Cooper Sq, New York, NY 10003, USA</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>24 Hour Fitness</v>
+      </c>
+      <c r="B21" t="str">
+        <v>https://www.24hourfitness.com/gyms/valley-stream-ny/valley-stream-green-acres-super-sport?Adb_id=GGL_LOC_ACQ_CDP</v>
+      </c>
+      <c r="C21" t="str">
+        <v>(516) 612-6119</v>
+      </c>
+      <c r="D21" t="str">
+        <v/>
+      </c>
+      <c r="E21">
+        <v>3.9</v>
+      </c>
+      <c r="F21" t="str">
+        <v>40.6628441, -73.727182</v>
+      </c>
+      <c r="G21" t="str">
+        <v>750 W Sunrise Hwy, Valley Stream, NY 11581, USA</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>New York Sports Club</v>
+      </c>
+      <c r="B22" t="str">
+        <v>https://www.newyorksportsclubs.com/clubs/23rd-park</v>
+      </c>
+      <c r="C22" t="str">
+        <v>(212) 982-4400</v>
+      </c>
+      <c r="D22" t="str">
+        <v/>
+      </c>
+      <c r="E22">
+        <v>4.4</v>
+      </c>
+      <c r="F22" t="str">
+        <v>40.7401753, -73.98571729999999</v>
+      </c>
+      <c r="G22" t="str">
+        <v>113 E 23rd St, New York, NY 10010, USA</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>CompleteBody Midtown East</v>
+      </c>
+      <c r="B23" t="str">
+        <v>https://www.completebody.com/completebody-midtown-east/</v>
+      </c>
+      <c r="C23" t="str">
+        <v>(212) 777-7703</v>
+      </c>
+      <c r="D23" t="str">
+        <v/>
+      </c>
+      <c r="E23">
+        <v>4.7</v>
+      </c>
+      <c r="F23" t="str">
+        <v>40.7593798, -73.9646707</v>
+      </c>
+      <c r="G23" t="str">
+        <v>301 E 57th St, New York, NY 10022, USA</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Mercedes Club</v>
+      </c>
+      <c r="B24" t="str">
+        <v>http://www.themercedesclub.com/</v>
+      </c>
+      <c r="C24" t="str">
+        <v>(212) 265-1111</v>
+      </c>
+      <c r="D24" t="str">
+        <v/>
+      </c>
+      <c r="E24">
+        <v>4.5</v>
+      </c>
+      <c r="F24" t="str">
+        <v>40.767725299999995, -73.9915642</v>
+      </c>
+      <c r="G24" t="str">
+        <v>550 W 54th St, New York, NY 10019, USA</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Planet Fitness</v>
+      </c>
+      <c r="B25" t="str">
+        <v>https://www.planetfitness.com/gyms/manhattan-canal-st-ny?utm_medium=organic&amp;utm_source=extnet</v>
+      </c>
+      <c r="C25" t="str">
+        <v>(646) 216-3031</v>
+      </c>
+      <c r="D25" t="str">
+        <v/>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25" t="str">
+        <v>40.7206893, -74.00435999999999</v>
+      </c>
+      <c r="G25" t="str">
+        <v>370 Canal St, New York, NY 10013, USA</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Crunch Fitness - 34th Street</v>
+      </c>
+      <c r="B26" t="str">
+        <v>https://www.crunch.com/locations/e-34th-st</v>
+      </c>
+      <c r="C26" t="str">
+        <v>(212) 545-9757</v>
+      </c>
+      <c r="D26" t="str">
+        <v/>
+      </c>
+      <c r="E26">
+        <v>3.4</v>
+      </c>
+      <c r="F26" t="str">
+        <v>40.7449717, -73.9770424</v>
+      </c>
+      <c r="G26" t="str">
+        <v>222 E 34th St, New York, NY 10016, USA</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Life Time</v>
+      </c>
+      <c r="B27" t="str">
+        <v>https://www.lifetime.life/locations/ny/battery-park.html?utm_source=google&amp;utm_medium=local&amp;utm_campaign=google-local-club</v>
+      </c>
+      <c r="C27" t="str">
+        <v>(212) 419-7300</v>
+      </c>
+      <c r="D27" t="str">
+        <v/>
+      </c>
+      <c r="E27">
+        <v>3.7</v>
+      </c>
+      <c r="F27" t="str">
+        <v>40.705242, -74.01612349999999</v>
+      </c>
+      <c r="G27" t="str">
+        <v>1 West St, New York, NY 10004, USA</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>New York Sports Club</v>
+      </c>
+      <c r="B28" t="str">
+        <v>https://www.newyorksportsclubs.com/clubs/murray-hill</v>
+      </c>
+      <c r="C28" t="str">
+        <v>(212) 686-1085</v>
+      </c>
+      <c r="D28" t="str">
+        <v/>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28" t="str">
+        <v>40.7465437, -73.980896</v>
+      </c>
+      <c r="G28" t="str">
+        <v>3 Park Ave, New York, NY 10016, USA</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Grind House Brooklyn</v>
+      </c>
+      <c r="B29" t="str">
+        <v>http://www.grindhousebk.com/</v>
+      </c>
+      <c r="C29" t="str">
+        <v>(718) 963-0835</v>
+      </c>
+      <c r="D29" t="str">
+        <v/>
+      </c>
+      <c r="E29">
+        <v>4.5</v>
+      </c>
+      <c r="F29" t="str">
+        <v>40.7164181, -73.961233</v>
+      </c>
+      <c r="G29" t="str">
+        <v>203 Berry St, Brooklyn, NY 11249, USA</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>CompleteBody 19th Street</v>
+      </c>
+      <c r="B30" t="str">
+        <v>https://www.completebody.com/completebody-19th-best-bodybuilding-gym-in-nyc/</v>
+      </c>
+      <c r="C30" t="str">
+        <v>(212) 777-7719</v>
+      </c>
+      <c r="D30" t="str">
+        <v/>
+      </c>
+      <c r="E30">
+        <v>4.7</v>
+      </c>
+      <c r="F30" t="str">
+        <v>40.7394932, -73.9928627</v>
+      </c>
+      <c r="G30" t="str">
+        <v>22 W 19th St, New York, NY 10011, USA</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Club 300 Tribeca - Luxury Gym | Personal Trainer</v>
+      </c>
+      <c r="B31" t="str">
+        <v>https://club300nyc.com/</v>
+      </c>
+      <c r="C31" t="str">
+        <v>(212) 575-1677</v>
+      </c>
+      <c r="D31" t="str">
+        <v/>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31" t="str">
+        <v>40.7168153, -74.0036685</v>
+      </c>
+      <c r="G31" t="str">
+        <v>101 Leonard St # Phb, New York, NY 10013, USA</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Powerhouse Gym Nanuet</v>
+      </c>
+      <c r="B32" t="str">
+        <v>http://www.powerhousegymnanuet.com/</v>
+      </c>
+      <c r="C32" t="str">
+        <v>(845) 501-4487</v>
+      </c>
+      <c r="D32" t="str">
+        <v/>
+      </c>
+      <c r="E32">
+        <v>4.6</v>
+      </c>
+      <c r="F32" t="str">
+        <v>41.0992606, -73.99927509999999</v>
+      </c>
+      <c r="G32" t="str">
+        <v>33 NY-304, Nanuet, NY 10954, USA</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Hype Gym Union Square</v>
+      </c>
+      <c r="B33" t="str">
+        <v>http://www.hypegym.com/</v>
+      </c>
+      <c r="C33" t="str">
+        <v>(646) 942-6754</v>
+      </c>
+      <c r="D33" t="str">
+        <v/>
+      </c>
+      <c r="E33">
+        <v>4.6</v>
+      </c>
+      <c r="F33" t="str">
+        <v>40.7370125, -73.9906051</v>
+      </c>
+      <c r="G33" t="str">
+        <v>37 Union Square W f2, New York, NY 10003, USA</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Oculus Fitness</v>
+      </c>
+      <c r="B34" t="str">
+        <v>http://www.oculusfitness.com/</v>
+      </c>
+      <c r="C34" t="str">
+        <v>(646) 832-4788</v>
+      </c>
+      <c r="D34" t="str">
+        <v/>
+      </c>
+      <c r="E34">
+        <v>4.9</v>
+      </c>
+      <c r="F34" t="str">
+        <v>40.7097951, -74.0063052</v>
+      </c>
+      <c r="G34" t="str">
+        <v>151 William St, New York, NY 10038, USA</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Manhattan Plaza Health Club</v>
+      </c>
+      <c r="B35" t="str">
+        <v>http://www.mphc.com/</v>
+      </c>
+      <c r="C35" t="str">
+        <v>(646) 590-4411</v>
+      </c>
+      <c r="D35" t="str">
+        <v/>
+      </c>
+      <c r="E35">
+        <v>4.2</v>
+      </c>
+      <c r="F35" t="str">
+        <v>40.7599419, -73.9946078</v>
+      </c>
+      <c r="G35" t="str">
+        <v>482 W 43rd St 2nd floor, New York, NY 10036, USA</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Planet Fitness</v>
+      </c>
+      <c r="B36" t="str">
+        <v>https://www.planetfitness.com/gyms/manhattan-harlem-125th-street-ny?utm_medium=organic&amp;utm_source=extnet</v>
+      </c>
+      <c r="C36" t="str">
+        <v>(212) 497-2644</v>
+      </c>
+      <c r="D36" t="str">
+        <v/>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36" t="str">
+        <v>40.80896, -73.94909</v>
+      </c>
+      <c r="G36" t="str">
+        <v>208 W 125th St, New York, NY 10027, USA</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Equinox Sports Club New York</v>
+      </c>
+      <c r="B37" t="str">
+        <v>https://www.equinox.com/clubs/new-york/uptown/sportsclubnewyork?cid=gmb</v>
+      </c>
+      <c r="C37" t="str">
+        <v>(212) 362-6800</v>
+      </c>
+      <c r="D37" t="str">
+        <v/>
+      </c>
+      <c r="E37">
+        <v>3.5</v>
+      </c>
+      <c r="F37" t="str">
+        <v>40.7745008, -73.9812756</v>
+      </c>
+      <c r="G37" t="str">
+        <v>160 Columbus Ave, New York, NY 10023, USA</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>SWEAT440 Fitness FiDi</v>
+      </c>
+      <c r="B38" t="str">
+        <v>https://sweat440.com/gyms/new-york/financial-district-10038/?utm_source=GMB&amp;utm_medium=organic&amp;utm_campaign=FiDi</v>
+      </c>
+      <c r="C38" t="str">
+        <v>(888) 507-9328</v>
+      </c>
+      <c r="D38" t="str">
+        <v/>
+      </c>
+      <c r="E38">
+        <v>4.9</v>
+      </c>
+      <c r="F38" t="str">
+        <v>40.708317799999996, -74.0068091</v>
+      </c>
+      <c r="G38" t="str">
+        <v>80 John St, New York, NY 10038, USA</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>CompleteBody Financial District</v>
+      </c>
+      <c r="B39" t="str">
+        <v>https://www.completebody.com/completebody-financial-district/</v>
+      </c>
+      <c r="C39" t="str">
+        <v>(212) 777-7702</v>
+      </c>
+      <c r="D39" t="str">
+        <v/>
+      </c>
+      <c r="E39">
+        <v>4.6</v>
+      </c>
+      <c r="F39" t="str">
+        <v>40.7046069, -74.0088274</v>
+      </c>
+      <c r="G39" t="str">
+        <v>10 Hanover Square, New York, NY 10005, USA</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Blink Fitness (PureGym)</v>
+      </c>
+      <c r="B40" t="str">
+        <v>https://www.puregym.com/us/gyms/ny/manhattan-noho</v>
+      </c>
+      <c r="C40" t="str">
+        <v>(212) 245-6008</v>
+      </c>
+      <c r="D40" t="str">
+        <v/>
+      </c>
+      <c r="E40">
+        <v>3.4</v>
+      </c>
+      <c r="F40" t="str">
+        <v>40.728133799999995, -73.9937135</v>
+      </c>
+      <c r="G40" t="str">
+        <v>16 E 4th St, New York, NY 10012, USA</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Crunch Fitness - Tribeca</v>
+      </c>
+      <c r="B41" t="str">
+        <v>https://www.crunch.com/locations/tribeca</v>
+      </c>
+      <c r="C41" t="str">
+        <v>(212) 966-5432</v>
+      </c>
+      <c r="D41" t="str">
+        <v/>
+      </c>
+      <c r="E41">
+        <v>3.9</v>
+      </c>
+      <c r="F41" t="str">
+        <v>40.7171327, -74.0051854</v>
+      </c>
+      <c r="G41" t="str">
+        <v>80 Leonard St, New York, NY 10013, USA</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>TMPL - West Village</v>
+      </c>
+      <c r="B42" t="str">
+        <v>https://www.tmplclubs.com/locations/tmpl-west-village?utm_source=google&amp;utm_medium=organic&amp;utm_campaign=google_my_business&amp;utm_id=west_village</v>
+      </c>
+      <c r="C42" t="str">
+        <v>(212) 206-1500</v>
+      </c>
+      <c r="D42" t="str">
+        <v/>
+      </c>
+      <c r="E42">
+        <v>4.6</v>
+      </c>
+      <c r="F42" t="str">
+        <v>40.734243, -74.0021848</v>
+      </c>
+      <c r="G42" t="str">
+        <v>125 7th Ave S, New York, NY 10014, USA</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>CrossFit Union Square</v>
+      </c>
+      <c r="B43" t="str">
+        <v>http://www.crossfitunionsquare.com/</v>
+      </c>
+      <c r="C43" t="str">
+        <v>(212) 254-9222</v>
+      </c>
+      <c r="D43" t="str">
+        <v/>
+      </c>
+      <c r="E43">
+        <v>4.8</v>
+      </c>
+      <c r="F43" t="str">
+        <v>40.7355333, -73.9918869</v>
+      </c>
+      <c r="G43" t="str">
+        <v>1 Union Square W Basement, New York, NY 10003, USA</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>The Lodge</v>
+      </c>
+      <c r="B44" t="str">
+        <v>http://www.thelodge-nyc.com/</v>
+      </c>
+      <c r="C44" t="str">
+        <v/>
+      </c>
+      <c r="D44" t="str">
+        <v/>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44" t="str">
+        <v>40.7232874, -74.0098075</v>
+      </c>
+      <c r="G44" t="str">
+        <v>450 Greenwich St, New York, NY 10013, USA</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>NYU 404 Fitness</v>
+      </c>
+      <c r="B45" t="str">
+        <v>https://gonyuathletics.com/sports/404-fitness</v>
+      </c>
+      <c r="C45" t="str">
+        <v>(212) 998-2020</v>
+      </c>
+      <c r="D45" t="str">
+        <v/>
+      </c>
+      <c r="E45">
+        <v>4.5</v>
+      </c>
+      <c r="F45" t="str">
+        <v>40.7284213, -73.99292319999999</v>
+      </c>
+      <c r="G45" t="str">
+        <v>404 Lafayette St, New York, NY 10003, USA</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>CrossFit Wall Street</v>
+      </c>
+      <c r="B46" t="str">
+        <v>http://crossfitwallstreet.com/</v>
+      </c>
+      <c r="C46" t="str">
+        <v>(646) 490-4244</v>
+      </c>
+      <c r="D46" t="str">
+        <v/>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46" t="str">
+        <v>40.7051289, -74.01246789999999</v>
+      </c>
+      <c r="G46" t="str">
+        <v>60 New St, New York, NY 10004, USA</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>CrossFit NYC</v>
+      </c>
+      <c r="B47" t="str">
+        <v>https://crossfitnyc.com/locations/gym-in-flatiron-new-york/</v>
+      </c>
+      <c r="C47" t="str">
+        <v>(212) 731-2165</v>
+      </c>
+      <c r="D47" t="str">
+        <v/>
+      </c>
+      <c r="E47">
+        <v>4.5</v>
+      </c>
+      <c r="F47" t="str">
+        <v>40.7457588, -73.99012689999999</v>
+      </c>
+      <c r="G47" t="str">
+        <v>50 W 28th St 2nd floor, New York, NY 10001, USA</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>SWEAT440 Fitness Chelsea</v>
+      </c>
+      <c r="B48" t="str">
+        <v>https://sweat440.com/gyms/new-york/chelsea-10011/?utm_source=GMB&amp;utm_medium=organic&amp;utm_campaign=chelsea</v>
+      </c>
+      <c r="C48" t="str">
+        <v>(888) 507-9328</v>
+      </c>
+      <c r="D48" t="str">
+        <v/>
+      </c>
+      <c r="E48">
+        <v>4.9</v>
+      </c>
+      <c r="F48" t="str">
+        <v>40.739371399999996, -73.99511389999999</v>
+      </c>
+      <c r="G48" t="str">
+        <v>600 6th Ave, New York, NY 10011, USA</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>GÜDSPORT at ARENA ONE</v>
+      </c>
+      <c r="B49" t="str">
+        <v>https://www.gudsport.net/</v>
+      </c>
+      <c r="C49" t="str">
+        <v>(917) 554-4490</v>
+      </c>
+      <c r="D49" t="str">
+        <v/>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49" t="str">
+        <v>40.7110759, -74.0120239</v>
+      </c>
+      <c r="G49" t="str">
+        <v>185 Greenwich St, New York, NY 10007, USA</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Gotham Gym</v>
+      </c>
+      <c r="B50" t="str">
+        <v>http://www.gothamgymnyc.com/</v>
+      </c>
+      <c r="C50" t="str">
+        <v>(646) 490-8500</v>
+      </c>
+      <c r="D50" t="str">
+        <v/>
+      </c>
+      <c r="E50">
+        <v>4.7</v>
+      </c>
+      <c r="F50" t="str">
+        <v>40.7306229, -74.0091815</v>
+      </c>
+      <c r="G50" t="str">
+        <v>600 Washington St, New York, NY 10014, USA</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>DOGPOUND Gym, Personal Training &amp; Group Fitness Classes</v>
+      </c>
+      <c r="B51" t="str">
+        <v>http://thedogpound.com/</v>
+      </c>
+      <c r="C51" t="str">
+        <v>(646) 620-6533</v>
+      </c>
+      <c r="D51" t="str">
+        <v/>
+      </c>
+      <c r="E51">
+        <v>4.8</v>
+      </c>
+      <c r="F51" t="str">
+        <v>40.7245092, -74.0087489</v>
+      </c>
+      <c r="G51" t="str">
+        <v>1 Renwick St, New York, NY 10013, USA</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>The Live Well Company</v>
+      </c>
+      <c r="B52" t="str">
+        <v/>
+      </c>
+      <c r="C52" t="str">
+        <v>(212) 431-5752</v>
+      </c>
+      <c r="D52" t="str">
+        <v/>
+      </c>
+      <c r="E52">
+        <v>5</v>
+      </c>
+      <c r="F52" t="str">
+        <v>40.7225034, -74.0112905</v>
+      </c>
+      <c r="G52" t="str">
+        <v>256 West St, New York, NY 10013, USA</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Orangetheory Fitness</v>
+      </c>
+      <c r="B53" t="str">
+        <v>https://www.orangetheory.com/en-us/locations/new-york-new-york-0894?utm_medium=seo&amp;utm_source=gg&amp;utm_term=corporate&amp;utm_campaign=soci</v>
+      </c>
+      <c r="C53" t="str">
+        <v>(646) 650-2122</v>
+      </c>
+      <c r="D53" t="str">
+        <v/>
+      </c>
+      <c r="E53">
+        <v>4.8</v>
+      </c>
+      <c r="F53" t="str">
+        <v>40.7084469, -74.0072574</v>
+      </c>
+      <c r="G53" t="str">
+        <v>100 William St, New York, NY 10038, USA</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>SoHo Strength Lab</v>
+      </c>
+      <c r="B54" t="str">
+        <v>http://sohostrengthlab.com/</v>
+      </c>
+      <c r="C54" t="str">
+        <v>(646) 926-1182</v>
+      </c>
+      <c r="D54" t="str">
+        <v/>
+      </c>
+      <c r="E54">
+        <v>4.9</v>
+      </c>
+      <c r="F54" t="str">
+        <v>40.7208447, -73.996426</v>
+      </c>
+      <c r="G54" t="str">
+        <v>182 Mulberry St, New York, NY 10012, USA</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>MCC Fitness</v>
+      </c>
+      <c r="B55" t="str">
+        <v>https://mannycantor.org/fitness</v>
+      </c>
+      <c r="C55" t="str">
+        <v>(646) 395-4285</v>
+      </c>
+      <c r="D55" t="str">
+        <v/>
+      </c>
+      <c r="E55">
+        <v>4.9</v>
+      </c>
+      <c r="F55" t="str">
+        <v>40.7139708, -73.9883747</v>
+      </c>
+      <c r="G55" t="str">
+        <v>197 E Broadway, New York, NY 10002, USA</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Crunch Fitness - Bowery</v>
+      </c>
+      <c r="B56" t="str">
+        <v>https://www.crunch.com/locations/bowery</v>
+      </c>
+      <c r="C56" t="str">
+        <v>(212) 614-0120</v>
+      </c>
+      <c r="D56" t="str">
+        <v/>
+      </c>
+      <c r="E56">
+        <v>3.9</v>
+      </c>
+      <c r="F56" t="str">
+        <v>40.7274856, -73.9917961</v>
+      </c>
+      <c r="G56" t="str">
+        <v>2 Cooper Sq, New York, NY 10003, USA</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Action Black Tribeca</v>
+      </c>
+      <c r="B57" t="str">
+        <v/>
+      </c>
+      <c r="C57" t="str">
+        <v>(347) 969-1354</v>
+      </c>
+      <c r="D57" t="str">
+        <v/>
+      </c>
+      <c r="E57">
+        <v>4.9</v>
+      </c>
+      <c r="F57" t="str">
+        <v>40.7194183, -74.0078633</v>
+      </c>
+      <c r="G57" t="str">
+        <v>152 Franklin St, New York, NY 10013, USA</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>F45 Training West Village</v>
+      </c>
+      <c r="B58" t="str">
+        <v>https://f45training.com/westvillage</v>
+      </c>
+      <c r="C58" t="str">
+        <v>(479) 800-1192</v>
+      </c>
+      <c r="D58" t="str">
+        <v/>
+      </c>
+      <c r="E58">
+        <v>4.8</v>
+      </c>
+      <c r="F58" t="str">
+        <v>40.729351199999996, -74.0049252</v>
+      </c>
+      <c r="G58" t="str">
+        <v>80 Carmine St, New York, NY 10014, USA</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Greenwich Village Athletic (GVA)</v>
+      </c>
+      <c r="B59" t="str">
+        <v>http://the-athleticclubs.com/greenwichvillageathletic</v>
+      </c>
+      <c r="C59" t="str">
+        <v>(347) 946-6381</v>
+      </c>
+      <c r="D59" t="str">
+        <v/>
+      </c>
+      <c r="E59">
+        <v>4.9</v>
+      </c>
+      <c r="F59" t="str">
+        <v>40.7266786, -73.9952904</v>
+      </c>
+      <c r="G59" t="str">
+        <v>650 Broadway, New York, NY 10012, USA</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>TMPL - Astor Place</v>
+      </c>
+      <c r="B60" t="str">
+        <v>https://www.tmplclubs.com/locations/tmpl-astor-place?utm_source=google&amp;utm_medium=organic&amp;utm_campaign=google_my_business&amp;utm_id=astor</v>
+      </c>
+      <c r="C60" t="str">
+        <v>(917) 877-1400</v>
+      </c>
+      <c r="D60" t="str">
+        <v/>
+      </c>
+      <c r="E60">
+        <v>4.4</v>
+      </c>
+      <c r="F60" t="str">
+        <v>40.7298469, -73.9924724</v>
+      </c>
+      <c r="G60" t="str">
+        <v>4 Astor Pl, New York, NY 10003, USA</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>Willspace</v>
+      </c>
+      <c r="B61" t="str">
+        <v>https://willspace.com/</v>
+      </c>
+      <c r="C61" t="str">
+        <v>(212) 929-1800</v>
+      </c>
+      <c r="D61" t="str">
+        <v/>
+      </c>
+      <c r="E61">
+        <v>4.9</v>
+      </c>
+      <c r="F61" t="str">
+        <v>40.7335393, -74.006511</v>
+      </c>
+      <c r="G61" t="str">
+        <v>513 Hudson St, New York, NY 10014, USA</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G61"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>